<commit_message>
dictionary final part - I
</commit_message>
<xml_diff>
--- a/teste-python-excel-shp/teste-excel-traduzido.xlsx
+++ b/teste-python-excel-shp/teste-excel-traduzido.xlsx
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SCEE SUL</t>
+          <t>SETOR DE CLUBES ESPORTIVOS E ESTÁDIOS SUL</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>SMI</t>
+          <t>SETOR DE MANSÕES ISOLADAS</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>SML</t>
+          <t>SETOR DE MANSÕES LAGO</t>
         </is>
       </c>
     </row>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>SHCAO</t>
+          <t>SETOR HABITACIONAL COLETIVO ÁREA OCTOGONAL</t>
         </is>
       </c>
     </row>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>SHJK</t>
+          <t>SETOR HABITACIONAL JUSCELINO KUBITSCHEK</t>
         </is>
       </c>
     </row>

</xml_diff>